<commit_message>
QC workflow has updated. New properties and classes are added under compliance form. QC and re-assignment are added under 'Reviews' collection  in compliance form. Able to request QC, and add comment
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_5.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_5.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Project Number</t>
   </si>
@@ -91,22 +91,10 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>Joseph williams</t>
-  </si>
-  <si>
-    <t>Joseph</t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
     <t>Role (PI/Sub I)</t>
   </si>
   <si>
     <t>PI</t>
-  </si>
-  <si>
-    <t>Sub I</t>
   </si>
   <si>
     <t>0910/0000</t>
@@ -524,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,19 +561,19 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -632,19 +620,19 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>22</v>
@@ -679,20 +667,6 @@
       </c>
       <c r="S2" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qc workflow is completed and is being tested
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_5.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -591,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -749,40 +749,29 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3">
-        <v>1122</v>
-      </c>
-      <c r="E3">
-        <v>2345</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -796,14 +785,20 @@
       <c r="E4">
         <v>2345</v>
       </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>39</v>
+      <c r="F4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -823,13 +818,13 @@
         <v>2345</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -849,15 +844,41 @@
         <v>2345</v>
       </c>
       <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>1122</v>
+      </c>
+      <c r="E7">
+        <v>2345</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
QCFailed and QCPassed has been replaced with QCCompleted. Tested Ok. Need to add two comments for QC inputs
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_5.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_5.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Project Number</t>
   </si>
@@ -158,6 +158,36 @@
   </si>
   <si>
     <t>Sub I</t>
+  </si>
+  <si>
+    <t>Huda, Syed</t>
+  </si>
+  <si>
+    <t>Syed</t>
+  </si>
+  <si>
+    <t>Huda</t>
+  </si>
+  <si>
+    <t>0000/0004</t>
+  </si>
+  <si>
+    <t>0000/0000</t>
+  </si>
+  <si>
+    <t>Liang, Cheng Yi</t>
+  </si>
+  <si>
+    <t>Yi</t>
+  </si>
+  <si>
+    <t>Liang</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
+    <t>St. Petersburg</t>
   </si>
 </sst>
 </file>
@@ -591,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,64 +732,66 @@
         <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="D2" s="7">
+        <v>9951</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" t="s">
+        <v>48</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="4" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="M2" s="5"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>889</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="7"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2274</v>
+      </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
+      <c r="I3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="4"/>
@@ -769,67 +801,80 @@
       <c r="R3" s="8"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4">
-        <v>1122</v>
-      </c>
-      <c r="E4">
-        <v>2345</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s">
-        <v>46</v>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>889</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>1122</v>
-      </c>
-      <c r="E5">
-        <v>2345</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -843,14 +888,20 @@
       <c r="E6">
         <v>2345</v>
       </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>41</v>
+      <c r="F6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -870,15 +921,67 @@
         <v>2345</v>
       </c>
       <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>1122</v>
+      </c>
+      <c r="E8">
+        <v>2345</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>1122</v>
+      </c>
+      <c r="E9">
+        <v>2345</v>
+      </c>
+      <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>